<commit_message>
added dlib face detections
</commit_message>
<xml_diff>
--- a/mediaeval/med17cross.xlsx
+++ b/mediaeval/med17cross.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">total sample</t>
   </si>
@@ -29,9 +29,15 @@
     <t xml:space="preserve">fear sample</t>
   </si>
   <si>
+    <t xml:space="preserve">Visual-feature-no</t>
+  </si>
+  <si>
     <t xml:space="preserve">extracted frames</t>
   </si>
   <si>
+    <t xml:space="preserve">approx.</t>
+  </si>
+  <si>
     <t xml:space="preserve">  'Decay': (912, 119),</t>
   </si>
   <si>
@@ -120,6 +126,36 @@
   </si>
   <si>
     <t xml:space="preserve">  'Payload': (214, 9),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, Left: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bottom: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frame width, height are 544, 1280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I found 1 face(s) in this photograph.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A face is located at pixel location </t>
+  </si>
+  <si>
+    <t xml:space="preserve">236 236 Ratio of face = 0.07998621323529412</t>
   </si>
 </sst>
 </file>
@@ -129,11 +165,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,138 +188,28 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -290,23 +217,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -330,153 +242,33 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -485,16 +277,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,10 +301,16 @@
       <c r="E1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>912</v>
@@ -527,7 +327,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>173</v>
@@ -538,7 +338,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>202</v>
@@ -549,7 +349,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>185</v>
@@ -560,7 +360,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>185</v>
@@ -581,7 +381,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>139</v>
@@ -592,7 +392,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>99</v>
@@ -603,7 +403,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>179</v>
@@ -614,7 +414,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>146</v>
@@ -625,13 +425,20 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>176</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>17</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>890</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">F16/5</f>
+        <v>178</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,7 +453,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>61</v>
@@ -657,7 +464,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>130</v>
@@ -668,7 +475,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>77</v>
@@ -679,7 +486,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>118</v>
@@ -690,7 +497,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>101</v>
@@ -701,7 +508,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>223</v>
@@ -726,7 +533,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>33</v>
@@ -734,17 +541,17 @@
       <c r="C27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="F27" s="0" t="n">
         <v>173</v>
       </c>
-      <c r="F27" s="0" t="n">
-        <f aca="false">E27/5</f>
+      <c r="G27" s="0" t="n">
+        <f aca="false">F27/5</f>
         <v>34.6</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>82</v>
@@ -755,7 +562,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>339</v>
@@ -766,7 +573,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>117</v>
@@ -774,10 +581,13 @@
       <c r="C30" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="E30" s="0" t="n">
+        <v>591</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>157</v>
@@ -802,7 +612,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>49</v>
@@ -813,7 +623,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>273</v>
@@ -821,10 +631,13 @@
       <c r="C35" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="E35" s="0" t="n">
+        <v>1374</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>155</v>
@@ -835,7 +648,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>227</v>
@@ -860,7 +673,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>127</v>
@@ -871,7 +684,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>22</v>
@@ -882,7 +695,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>176</v>
@@ -890,10 +703,13 @@
       <c r="C42" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="E42" s="0" t="n">
+        <v>888</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>197</v>
@@ -901,10 +717,13 @@
       <c r="C43" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="E43" s="0" t="n">
+        <v>990</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>214</v>
@@ -939,17 +758,111 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.72"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>544</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1280</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">E2-C2</f>
+        <v>544</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">F2-D2</f>
+        <v>1280</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">G2*H2</f>
+        <v>696320</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>237</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>423</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>473</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">E3-C3</f>
+        <v>236</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">F3-D3</f>
+        <v>236</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">G3*H3</f>
+        <v>55696</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">I3/I2</f>
+        <v>0.0799862132352941</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>